<commit_message>
Add Function Points into UseCaseDoc
</commit_message>
<xml_diff>
--- a/SE2_Week 2/Usecase doc.xlsx
+++ b/SE2_Week 2/Usecase doc.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="36">
   <si>
     <t>UC</t>
   </si>
@@ -87,16 +87,7 @@
     <t>17h</t>
   </si>
   <si>
-    <t>27h</t>
-  </si>
-  <si>
     <t>4,5h</t>
-  </si>
-  <si>
-    <t>7,5h</t>
-  </si>
-  <si>
-    <t>2,5h</t>
   </si>
   <si>
     <t>9h</t>
@@ -138,8 +129,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -163,6 +154,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -602,7 +600,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -662,9 +660,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
@@ -677,14 +672,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -694,19 +693,30 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Link" xfId="1" builtinId="8"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -722,10 +732,210 @@
 </styleSheet>
 </file>
 
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="de-DE"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Tabelle1!$I$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>FP</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:trendline>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Tabelle1!$H$3:$H$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7.5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Tabelle1!$I$3:$I$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>102.6</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>50.92</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>40.28</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>34.96</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>24.32</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="58056064"/>
+        <c:axId val="58054528"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="58056064"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines/>
+        <c:minorGridlines/>
+        <c:title>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="58054528"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="58054528"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:minorGridlines/>
+        <c:title>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="58056064"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.7" r="0.7" t="0.78740157499999996" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>157162</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>14287</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Diagramm 4"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Larissa">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -763,9 +973,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Larissa">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -800,7 +1010,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -835,7 +1045,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Larissa">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1015,7 +1225,7 @@
   <dimension ref="C1:K25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N24" sqref="N24"/>
+      <selection activeCell="M18" sqref="M18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1047,7 +1257,7 @@
       <c r="I2" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="K2" s="42"/>
+      <c r="K2" s="34"/>
     </row>
     <row r="3" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C3" s="9">
@@ -1065,10 +1275,12 @@
       <c r="G3" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="H3" s="22" t="s">
-        <v>23</v>
-      </c>
-      <c r="I3" s="18"/>
+      <c r="H3" s="22">
+        <v>27</v>
+      </c>
+      <c r="I3" s="18">
+        <v>102.6</v>
+      </c>
     </row>
     <row r="4" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C4" s="10">
@@ -1078,18 +1290,20 @@
         <v>8</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="G4" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="H4" s="23" t="s">
-        <v>23</v>
-      </c>
-      <c r="I4" s="19"/>
+      <c r="H4" s="23">
+        <v>27</v>
+      </c>
+      <c r="I4" s="19">
+        <v>50.92</v>
+      </c>
     </row>
     <row r="5" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C5" s="10">
@@ -1107,10 +1321,12 @@
       <c r="G5" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="H5" s="23" t="s">
-        <v>15</v>
-      </c>
-      <c r="I5" s="19"/>
+      <c r="H5" s="23">
+        <v>2</v>
+      </c>
+      <c r="I5" s="20">
+        <v>40.28</v>
+      </c>
     </row>
     <row r="6" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C6" s="10">
@@ -1123,15 +1339,17 @@
         <v>15</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G6" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="H6" s="23" t="s">
-        <v>25</v>
-      </c>
-      <c r="I6" s="19"/>
+      <c r="H6" s="23">
+        <v>7.5</v>
+      </c>
+      <c r="I6" s="19">
+        <v>34.96</v>
+      </c>
     </row>
     <row r="7" spans="3:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C7" s="11">
@@ -1149,36 +1367,38 @@
       <c r="G7" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="H7" s="24" t="s">
-        <v>26</v>
-      </c>
-      <c r="I7" s="20"/>
+      <c r="H7" s="24">
+        <v>2.5</v>
+      </c>
+      <c r="I7" s="20">
+        <v>24.32</v>
+      </c>
     </row>
     <row r="8" spans="3:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C8" s="38" t="s">
+      <c r="C8" s="37" t="s">
         <v>20</v>
       </c>
-      <c r="D8" s="39"/>
-      <c r="E8" s="39"/>
-      <c r="F8" s="39"/>
-      <c r="G8" s="39"/>
-      <c r="H8" s="39"/>
-      <c r="I8" s="40"/>
+      <c r="D8" s="38"/>
+      <c r="E8" s="38"/>
+      <c r="F8" s="38"/>
+      <c r="G8" s="38"/>
+      <c r="H8" s="38"/>
+      <c r="I8" s="39"/>
     </row>
     <row r="9" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C9" s="28">
+      <c r="C9" s="27">
         <v>6</v>
       </c>
-      <c r="D9" s="29" t="s">
+      <c r="D9" s="28" t="s">
         <v>12</v>
       </c>
-      <c r="E9" s="30" t="s">
+      <c r="E9" s="29" t="s">
         <v>15</v>
       </c>
-      <c r="F9" s="30"/>
-      <c r="G9" s="31"/>
-      <c r="H9" s="25"/>
-      <c r="I9" s="32"/>
+      <c r="F9" s="29"/>
+      <c r="G9" s="30"/>
+      <c r="H9" s="40"/>
+      <c r="I9" s="41"/>
     </row>
     <row r="10" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C10" s="10">
@@ -1192,8 +1412,8 @@
       </c>
       <c r="F10" s="2"/>
       <c r="G10" s="15"/>
-      <c r="H10" s="23"/>
-      <c r="I10" s="19"/>
+      <c r="H10" s="42"/>
+      <c r="I10" s="43"/>
     </row>
     <row r="11" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C11" s="10">
@@ -1207,130 +1427,132 @@
       </c>
       <c r="F11" s="2"/>
       <c r="G11" s="15"/>
-      <c r="H11" s="23"/>
-      <c r="I11" s="19"/>
+      <c r="H11" s="42"/>
+      <c r="I11" s="43"/>
     </row>
     <row r="12" spans="3:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C12" s="33">
+      <c r="C12" s="31">
         <v>9</v>
       </c>
-      <c r="D12" s="34" t="s">
-        <v>29</v>
-      </c>
-      <c r="E12" s="41" t="s">
+      <c r="D12" s="32" t="s">
+        <v>26</v>
+      </c>
+      <c r="E12" s="33" t="s">
         <v>16</v>
       </c>
-      <c r="F12" s="34"/>
-      <c r="G12" s="35"/>
-      <c r="H12" s="36"/>
-      <c r="I12" s="37"/>
+      <c r="F12" s="33"/>
+      <c r="G12" s="44"/>
+      <c r="H12" s="45"/>
+      <c r="I12" s="46">
+        <v>20.52</v>
+      </c>
     </row>
     <row r="13" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C13" s="26"/>
-      <c r="D13" s="27"/>
-      <c r="E13" s="27"/>
-      <c r="F13" s="27"/>
-      <c r="G13" s="27"/>
-      <c r="H13" s="27"/>
-      <c r="I13" s="27"/>
+      <c r="C13" s="25"/>
+      <c r="D13" s="26"/>
+      <c r="E13" s="26"/>
+      <c r="F13" s="26"/>
+      <c r="G13" s="26"/>
+      <c r="H13" s="26"/>
+      <c r="I13" s="26"/>
     </row>
     <row r="17" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C17" s="43" t="s">
+      <c r="C17" s="35" t="s">
         <v>0</v>
       </c>
       <c r="D17" t="s">
         <v>7</v>
       </c>
-      <c r="E17" s="44" t="s">
-        <v>30</v>
+      <c r="E17" s="36" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="18" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C18" s="43" t="s">
+      <c r="C18" s="35" t="s">
         <v>0</v>
       </c>
       <c r="D18" t="s">
         <v>8</v>
       </c>
-      <c r="E18" s="44" t="s">
-        <v>31</v>
+      <c r="E18" s="36" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="19" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C19" s="43" t="s">
+      <c r="C19" s="35" t="s">
         <v>0</v>
       </c>
       <c r="D19" t="s">
         <v>9</v>
       </c>
-      <c r="E19" s="44" t="s">
-        <v>32</v>
+      <c r="E19" s="36" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="20" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C20" s="43" t="s">
+      <c r="C20" s="35" t="s">
         <v>0</v>
       </c>
       <c r="D20" t="s">
         <v>10</v>
       </c>
-      <c r="E20" s="44" t="s">
-        <v>33</v>
+      <c r="E20" s="36" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="21" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C21" s="43" t="s">
+      <c r="C21" s="35" t="s">
         <v>0</v>
       </c>
       <c r="D21" t="s">
         <v>11</v>
       </c>
-      <c r="E21" s="44" t="s">
-        <v>34</v>
+      <c r="E21" s="36" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="22" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C22" s="43" t="s">
+      <c r="C22" s="35" t="s">
         <v>0</v>
       </c>
       <c r="D22" t="s">
         <v>12</v>
       </c>
-      <c r="E22" s="44" t="s">
-        <v>35</v>
+      <c r="E22" s="36" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="23" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C23" s="43" t="s">
+      <c r="C23" s="35" t="s">
         <v>0</v>
       </c>
       <c r="D23" t="s">
         <v>13</v>
       </c>
-      <c r="E23" s="44" t="s">
-        <v>36</v>
+      <c r="E23" s="36" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="24" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C24" s="43" t="s">
+      <c r="C24" s="35" t="s">
         <v>0</v>
       </c>
       <c r="D24" t="s">
         <v>14</v>
       </c>
-      <c r="E24" s="44" t="s">
-        <v>37</v>
+      <c r="E24" s="36" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="25" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C25" s="43" t="s">
+      <c r="C25" s="35" t="s">
         <v>0</v>
       </c>
       <c r="D25" t="s">
-        <v>29</v>
-      </c>
-      <c r="E25" s="44" t="s">
-        <v>38</v>
+        <v>26</v>
+      </c>
+      <c r="E25" s="36" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -1350,6 +1572,7 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="landscape" r:id="rId10"/>
+  <drawing r:id="rId11"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Update UseCase doc with FP
</commit_message>
<xml_diff>
--- a/SE2_Week 2/Usecase doc.xlsx
+++ b/SE2_Week 2/Usecase doc.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="28">
   <si>
     <t>UC</t>
   </si>
@@ -63,39 +63,9 @@
     <t>View Statistic</t>
   </si>
   <si>
-    <t>2h</t>
-  </si>
-  <si>
-    <t>0,5h</t>
-  </si>
-  <si>
-    <t>1h</t>
-  </si>
-  <si>
-    <t>1,5h</t>
-  </si>
-  <si>
-    <t>3h</t>
-  </si>
-  <si>
     <t>SEMESTERBREAK</t>
   </si>
   <si>
-    <t>7h</t>
-  </si>
-  <si>
-    <t>17h</t>
-  </si>
-  <si>
-    <t>4,5h</t>
-  </si>
-  <si>
-    <t>9h</t>
-  </si>
-  <si>
-    <t>17,5h</t>
-  </si>
-  <si>
     <t>Extend Settings</t>
   </si>
   <si>
@@ -126,19 +96,16 @@
     <t>https://github.com/nappydevelopment/docs/blob/master/pdfs/9%20UseCase_Extend_Settings.pdf</t>
   </si>
   <si>
-    <t>56.88</t>
-  </si>
-  <si>
     <t>*</t>
   </si>
   <si>
-    <t>* nur eine Schätzung da Anzahl "Numer of User Inquiries" immer unterschiedlich</t>
+    <t>* nur eine Schätzung da "Numer of User Inquiries" immer unterschiedlich</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -609,17 +576,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -632,21 +593,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -661,31 +610,13 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -693,27 +624,13 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -723,16 +640,60 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="4" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Link" xfId="1" builtinId="8"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -749,7 +710,7 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="de-DE"/>
   <c:roundedCorners val="0"/>
@@ -796,22 +757,22 @@
             <c:numRef>
               <c:f>Tabelle1!$H$3:$H$7</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>27</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>27</c:v>
+                  <c:v>27.5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>7.5</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.5</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -823,13 +784,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>66.36</c:v>
+                  <c:v>78.37</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>62.41</c:v>
+                  <c:v>72.41</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>53.88</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>41.08</c:v>
@@ -841,7 +802,7 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-684E-462E-B6C5-08C4C156CB9E}"/>
             </c:ext>
@@ -855,11 +816,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="58056064"/>
-        <c:axId val="58054528"/>
+        <c:axId val="67871872"/>
+        <c:axId val="67873792"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="58056064"/>
+        <c:axId val="67871872"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -868,19 +829,34 @@
         <c:majorGridlines/>
         <c:minorGridlines/>
         <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="de-DE"/>
+                  <a:t>Total time</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
           <c:layout/>
           <c:overlay val="0"/>
         </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="58054528"/>
+        <c:crossAx val="67873792"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="58054528"/>
+        <c:axId val="67873792"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -889,6 +865,21 @@
         <c:majorGridlines/>
         <c:minorGridlines/>
         <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="de-DE"/>
+                  <a:t>FP</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
           <c:layout/>
           <c:overlay val="0"/>
         </c:title>
@@ -896,7 +887,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="58056064"/>
+        <c:crossAx val="67871872"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -923,15 +914,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:colOff>285749</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>157162</xdr:rowOff>
+      <xdr:rowOff>4762</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>14287</xdr:rowOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>66674</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -954,9 +945,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Larissa">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -994,9 +985,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Larissa">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1031,7 +1022,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1066,7 +1057,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Larissa">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1246,7 +1237,7 @@
   <dimension ref="C1:K25"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="N22" sqref="N22"/>
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1257,348 +1248,353 @@
   <sheetData>
     <row r="1" spans="3:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="3:11" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="D2" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="8" t="s">
+      <c r="E2" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="8" t="s">
+      <c r="F2" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="13" t="s">
+      <c r="G2" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="H2" s="21" t="s">
+      <c r="H2" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="I2" s="17" t="s">
+      <c r="I2" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="K2" s="34"/>
+      <c r="K2" s="22"/>
     </row>
     <row r="3" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C3" s="9">
+      <c r="C3" s="7">
         <v>1</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D3" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="F3" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="G3" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="H3" s="22">
+      <c r="E3" s="31">
+        <v>3</v>
+      </c>
+      <c r="F3" s="31">
+        <v>17</v>
+      </c>
+      <c r="G3" s="32">
+        <v>7</v>
+      </c>
+      <c r="H3" s="37">
+        <f>E3+F3+G3</f>
         <v>27</v>
       </c>
-      <c r="I3" s="18">
-        <v>66.36</v>
-      </c>
-      <c r="J3" s="48" t="s">
-        <v>37</v>
+      <c r="I3" s="12">
+        <v>78.37</v>
+      </c>
+      <c r="J3" s="26" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="4" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C4" s="10">
+      <c r="C4" s="8">
         <v>2</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E4" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="G4" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="H4" s="23">
-        <v>27</v>
-      </c>
-      <c r="I4" s="19">
-        <v>62.41</v>
+      <c r="E4" s="33">
+        <v>17.5</v>
+      </c>
+      <c r="F4" s="33">
+        <v>9</v>
+      </c>
+      <c r="G4" s="34">
+        <v>1</v>
+      </c>
+      <c r="H4" s="37">
+        <f t="shared" ref="H4:H7" si="0">E4+F4+G4</f>
+        <v>27.5</v>
+      </c>
+      <c r="I4" s="13">
+        <v>72.41</v>
       </c>
     </row>
     <row r="5" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C5" s="10">
+      <c r="C5" s="8">
         <v>3</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E5" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="G5" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="H5" s="23">
-        <v>4</v>
-      </c>
-      <c r="I5" s="20" t="s">
-        <v>36</v>
+      <c r="E5" s="33">
+        <v>1</v>
+      </c>
+      <c r="F5" s="33">
+        <v>7</v>
+      </c>
+      <c r="G5" s="34">
+        <v>1</v>
+      </c>
+      <c r="H5" s="37">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="I5" s="14">
+        <v>53.88</v>
       </c>
     </row>
     <row r="6" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C6" s="10">
+      <c r="C6" s="8">
         <v>4</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E6" s="2" t="s">
+      <c r="E6" s="33">
+        <v>2</v>
+      </c>
+      <c r="F6" s="33">
+        <v>4.5</v>
+      </c>
+      <c r="G6" s="34">
+        <v>1</v>
+      </c>
+      <c r="H6" s="37">
+        <f t="shared" si="0"/>
+        <v>7.5</v>
+      </c>
+      <c r="I6" s="13">
+        <v>41.08</v>
+      </c>
+    </row>
+    <row r="7" spans="3:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C7" s="9">
+        <v>5</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E7" s="35">
+        <v>1</v>
+      </c>
+      <c r="F7" s="35">
+        <v>4.5</v>
+      </c>
+      <c r="G7" s="36">
+        <v>0.5</v>
+      </c>
+      <c r="H7" s="37">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="I7" s="25">
+        <v>25.28</v>
+      </c>
+    </row>
+    <row r="8" spans="3:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C8" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="F6" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="G6" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="H6" s="23">
-        <v>7.5</v>
-      </c>
-      <c r="I6" s="19">
-        <v>41.08</v>
-      </c>
-    </row>
-    <row r="7" spans="3:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C7" s="11">
-        <v>5</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E7" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="F7" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="G7" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="H7" s="24">
-        <v>2.5</v>
-      </c>
-      <c r="I7" s="47">
-        <v>25.28</v>
-      </c>
-    </row>
-    <row r="8" spans="3:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C8" s="44" t="s">
-        <v>20</v>
-      </c>
-      <c r="D8" s="45"/>
-      <c r="E8" s="45"/>
-      <c r="F8" s="45"/>
-      <c r="G8" s="45"/>
-      <c r="H8" s="45"/>
-      <c r="I8" s="46"/>
+      <c r="D8" s="29"/>
+      <c r="E8" s="29"/>
+      <c r="F8" s="29"/>
+      <c r="G8" s="29"/>
+      <c r="H8" s="29"/>
+      <c r="I8" s="30"/>
     </row>
     <row r="9" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C9" s="27">
+      <c r="C9" s="18">
         <v>6</v>
       </c>
-      <c r="D9" s="28" t="s">
+      <c r="D9" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="E9" s="29" t="s">
-        <v>15</v>
-      </c>
-      <c r="F9" s="29"/>
-      <c r="G9" s="30"/>
-      <c r="H9" s="37">
-        <v>30</v>
-      </c>
-      <c r="I9" s="38">
+      <c r="E9" s="38">
+        <v>2</v>
+      </c>
+      <c r="F9" s="38"/>
+      <c r="G9" s="39"/>
+      <c r="H9" s="40">
+        <v>25</v>
+      </c>
+      <c r="I9" s="41">
         <v>71.099999999999994</v>
       </c>
       <c r="J9" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
     </row>
     <row r="10" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C10" s="10">
+      <c r="C10" s="8">
         <v>7</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E10" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="F10" s="2"/>
-      <c r="G10" s="15"/>
-      <c r="H10" s="39">
-        <v>9</v>
-      </c>
-      <c r="I10" s="40">
+      <c r="E10" s="33">
+        <v>1</v>
+      </c>
+      <c r="F10" s="33"/>
+      <c r="G10" s="34"/>
+      <c r="H10" s="42">
+        <v>5</v>
+      </c>
+      <c r="I10" s="43">
         <v>30.81</v>
       </c>
     </row>
     <row r="11" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C11" s="10">
+      <c r="C11" s="8">
         <v>8</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E11" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="F11" s="2"/>
-      <c r="G11" s="15"/>
-      <c r="H11" s="39">
-        <v>17</v>
-      </c>
-      <c r="I11" s="40">
+      <c r="E11" s="33">
+        <v>1</v>
+      </c>
+      <c r="F11" s="33"/>
+      <c r="G11" s="34"/>
+      <c r="H11" s="42">
+        <v>11</v>
+      </c>
+      <c r="I11" s="43">
         <v>45.03</v>
       </c>
     </row>
     <row r="12" spans="3:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C12" s="31">
+      <c r="C12" s="20">
         <v>9</v>
       </c>
-      <c r="D12" s="32" t="s">
-        <v>26</v>
-      </c>
-      <c r="E12" s="33" t="s">
+      <c r="D12" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="F12" s="33"/>
-      <c r="G12" s="41"/>
-      <c r="H12" s="42">
-        <v>5</v>
-      </c>
-      <c r="I12" s="43">
+      <c r="E12" s="44">
+        <v>0.5</v>
+      </c>
+      <c r="F12" s="44"/>
+      <c r="G12" s="45"/>
+      <c r="H12" s="46">
+        <v>2</v>
+      </c>
+      <c r="I12" s="47">
         <v>23.7</v>
       </c>
     </row>
     <row r="13" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C13" s="25"/>
-      <c r="D13" s="26"/>
-      <c r="E13" s="26"/>
-      <c r="F13" s="26"/>
-      <c r="G13" s="26"/>
-      <c r="H13" s="26"/>
-      <c r="I13" s="26"/>
+      <c r="C13" s="16"/>
+      <c r="D13" s="17"/>
+      <c r="E13" s="17"/>
+      <c r="F13" s="17"/>
+      <c r="G13" s="17"/>
+      <c r="H13" s="17"/>
+      <c r="I13" s="17"/>
     </row>
     <row r="14" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="D14" s="49" t="s">
-        <v>38</v>
+      <c r="D14" s="27" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="17" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C17" s="35" t="s">
+      <c r="C17" s="23" t="s">
         <v>0</v>
       </c>
       <c r="D17" t="s">
         <v>7</v>
       </c>
-      <c r="E17" s="36" t="s">
-        <v>27</v>
+      <c r="E17" s="24" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="18" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C18" s="35" t="s">
+      <c r="C18" s="23" t="s">
         <v>0</v>
       </c>
       <c r="D18" t="s">
         <v>8</v>
       </c>
-      <c r="E18" s="36" t="s">
-        <v>28</v>
+      <c r="E18" s="24" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="19" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C19" s="35" t="s">
+      <c r="C19" s="23" t="s">
         <v>0</v>
       </c>
       <c r="D19" t="s">
         <v>9</v>
       </c>
-      <c r="E19" s="36" t="s">
-        <v>29</v>
+      <c r="E19" s="24" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="20" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C20" s="35" t="s">
+      <c r="C20" s="23" t="s">
         <v>0</v>
       </c>
       <c r="D20" t="s">
         <v>10</v>
       </c>
-      <c r="E20" s="36" t="s">
-        <v>30</v>
+      <c r="E20" s="24" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="21" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C21" s="35" t="s">
+      <c r="C21" s="23" t="s">
         <v>0</v>
       </c>
       <c r="D21" t="s">
         <v>11</v>
       </c>
-      <c r="E21" s="36" t="s">
-        <v>31</v>
+      <c r="E21" s="24" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="22" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C22" s="35" t="s">
+      <c r="C22" s="23" t="s">
         <v>0</v>
       </c>
       <c r="D22" t="s">
         <v>12</v>
       </c>
-      <c r="E22" s="36" t="s">
-        <v>32</v>
+      <c r="E22" s="24" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="23" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C23" s="35" t="s">
+      <c r="C23" s="23" t="s">
         <v>0</v>
       </c>
       <c r="D23" t="s">
         <v>13</v>
       </c>
-      <c r="E23" s="36" t="s">
-        <v>33</v>
+      <c r="E23" s="24" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="24" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C24" s="35" t="s">
+      <c r="C24" s="23" t="s">
         <v>0</v>
       </c>
       <c r="D24" t="s">
         <v>14</v>
       </c>
-      <c r="E24" s="36" t="s">
-        <v>34</v>
+      <c r="E24" s="24" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="25" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C25" s="35" t="s">
+      <c r="C25" s="23" t="s">
         <v>0</v>
       </c>
       <c r="D25" t="s">
-        <v>26</v>
-      </c>
-      <c r="E25" s="36" t="s">
-        <v>35</v>
+        <v>16</v>
+      </c>
+      <c r="E25" s="24" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add FP estimation into UC
</commit_message>
<xml_diff>
--- a/SE2_Week 2/Usecase doc.xlsx
+++ b/SE2_Week 2/Usecase doc.xlsx
@@ -631,6 +631,57 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -639,57 +690,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -816,11 +816,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="67871872"/>
-        <c:axId val="67873792"/>
+        <c:axId val="67224704"/>
+        <c:axId val="67226624"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="67871872"/>
+        <c:axId val="67224704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -851,12 +851,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="67873792"/>
+        <c:crossAx val="67226624"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="67873792"/>
+        <c:axId val="67226624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -887,7 +887,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="67871872"/>
+        <c:crossAx val="67224704"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1237,7 +1237,7 @@
   <dimension ref="C1:K25"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+      <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1278,16 +1278,16 @@
       <c r="D3" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="31">
+      <c r="E3" s="28">
         <v>3</v>
       </c>
-      <c r="F3" s="31">
+      <c r="F3" s="28">
         <v>17</v>
       </c>
-      <c r="G3" s="32">
+      <c r="G3" s="29">
         <v>7</v>
       </c>
-      <c r="H3" s="37">
+      <c r="H3" s="34">
         <f>E3+F3+G3</f>
         <v>27</v>
       </c>
@@ -1305,16 +1305,16 @@
       <c r="D4" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E4" s="33">
+      <c r="E4" s="30">
         <v>17.5</v>
       </c>
-      <c r="F4" s="33">
+      <c r="F4" s="30">
         <v>9</v>
       </c>
-      <c r="G4" s="34">
+      <c r="G4" s="31">
         <v>1</v>
       </c>
-      <c r="H4" s="37">
+      <c r="H4" s="34">
         <f t="shared" ref="H4:H7" si="0">E4+F4+G4</f>
         <v>27.5</v>
       </c>
@@ -1329,16 +1329,16 @@
       <c r="D5" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E5" s="33">
+      <c r="E5" s="30">
         <v>1</v>
       </c>
-      <c r="F5" s="33">
+      <c r="F5" s="30">
         <v>7</v>
       </c>
-      <c r="G5" s="34">
+      <c r="G5" s="31">
         <v>1</v>
       </c>
-      <c r="H5" s="37">
+      <c r="H5" s="34">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
@@ -1353,16 +1353,16 @@
       <c r="D6" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E6" s="33">
+      <c r="E6" s="30">
         <v>2</v>
       </c>
-      <c r="F6" s="33">
+      <c r="F6" s="30">
         <v>4.5</v>
       </c>
-      <c r="G6" s="34">
+      <c r="G6" s="31">
         <v>1</v>
       </c>
-      <c r="H6" s="37">
+      <c r="H6" s="34">
         <f t="shared" si="0"/>
         <v>7.5</v>
       </c>
@@ -1377,16 +1377,16 @@
       <c r="D7" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E7" s="35">
+      <c r="E7" s="32">
         <v>1</v>
       </c>
-      <c r="F7" s="35">
+      <c r="F7" s="32">
         <v>4.5</v>
       </c>
-      <c r="G7" s="36">
+      <c r="G7" s="33">
         <v>0.5</v>
       </c>
-      <c r="H7" s="37">
+      <c r="H7" s="34">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
@@ -1395,15 +1395,15 @@
       </c>
     </row>
     <row r="8" spans="3:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C8" s="28" t="s">
+      <c r="C8" s="45" t="s">
         <v>15</v>
       </c>
-      <c r="D8" s="29"/>
-      <c r="E8" s="29"/>
-      <c r="F8" s="29"/>
-      <c r="G8" s="29"/>
-      <c r="H8" s="29"/>
-      <c r="I8" s="30"/>
+      <c r="D8" s="46"/>
+      <c r="E8" s="46"/>
+      <c r="F8" s="46"/>
+      <c r="G8" s="46"/>
+      <c r="H8" s="46"/>
+      <c r="I8" s="47"/>
     </row>
     <row r="9" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C9" s="18">
@@ -1412,15 +1412,15 @@
       <c r="D9" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="E9" s="38">
+      <c r="E9" s="35">
         <v>2</v>
       </c>
-      <c r="F9" s="38"/>
-      <c r="G9" s="39"/>
-      <c r="H9" s="40">
+      <c r="F9" s="35"/>
+      <c r="G9" s="36"/>
+      <c r="H9" s="37">
         <v>25</v>
       </c>
-      <c r="I9" s="41">
+      <c r="I9" s="38">
         <v>71.099999999999994</v>
       </c>
       <c r="J9" t="s">
@@ -1434,15 +1434,15 @@
       <c r="D10" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E10" s="33">
+      <c r="E10" s="30">
         <v>1</v>
       </c>
-      <c r="F10" s="33"/>
-      <c r="G10" s="34"/>
-      <c r="H10" s="42">
+      <c r="F10" s="30"/>
+      <c r="G10" s="31"/>
+      <c r="H10" s="39">
         <v>5</v>
       </c>
-      <c r="I10" s="43">
+      <c r="I10" s="40">
         <v>30.81</v>
       </c>
     </row>
@@ -1453,15 +1453,15 @@
       <c r="D11" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E11" s="33">
+      <c r="E11" s="30">
         <v>1</v>
       </c>
-      <c r="F11" s="33"/>
-      <c r="G11" s="34"/>
-      <c r="H11" s="42">
+      <c r="F11" s="30"/>
+      <c r="G11" s="31"/>
+      <c r="H11" s="39">
         <v>11</v>
       </c>
-      <c r="I11" s="43">
+      <c r="I11" s="40">
         <v>45.03</v>
       </c>
     </row>
@@ -1472,15 +1472,15 @@
       <c r="D12" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="E12" s="44">
+      <c r="E12" s="41">
         <v>0.5</v>
       </c>
-      <c r="F12" s="44"/>
-      <c r="G12" s="45"/>
-      <c r="H12" s="46">
+      <c r="F12" s="41"/>
+      <c r="G12" s="42"/>
+      <c r="H12" s="43">
         <v>2</v>
       </c>
-      <c r="I12" s="47">
+      <c r="I12" s="44">
         <v>23.7</v>
       </c>
     </row>

</xml_diff>